<commit_message>
Updating STM Interface board to latest rev.
</commit_message>
<xml_diff>
--- a/stm32_interface_board/Ordering/stm32_interface_board.xlsx
+++ b/stm32_interface_board/Ordering/stm32_interface_board.xlsx
@@ -586,7 +586,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
   <si>
     <t xml:space="preserve">Board Qty:</t>
   </si>
@@ -738,6 +738,21 @@
     <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x03</t>
   </si>
   <si>
+    <t xml:space="preserve">61300311021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-5336-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2356177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-61300311021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">828-1654</t>
+  </si>
+  <si>
     <t xml:space="preserve">U3</t>
   </si>
   <si>
@@ -810,7 +825,7 @@
     <t xml:space="preserve">44X3416</t>
   </si>
   <si>
-    <t xml:space="preserve">TH1-TH3</t>
+    <t xml:space="preserve">TH1-TH4</t>
   </si>
   <si>
     <t xml:space="preserve">PTH</t>
@@ -1264,7 +1279,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1294,7 +1309,7 @@
     <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1302,25 +1317,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">SUM(I7:I22)</f>
-        <v>130.07801</v>
+        <v>135.39265</v>
       </c>
       <c r="M2" s="3" t="n">
         <f aca="false">SUM(M7:M22)</f>
-        <v>142.276</v>
+        <v>149.276</v>
       </c>
       <c r="S2" s="3" t="n">
         <f aca="false">SUM(S7:S22)</f>
-        <v>38.83116</v>
+        <v>44.1458</v>
       </c>
       <c r="Y2" s="3" t="n">
         <f aca="false">SUM(Y7:Y22)</f>
-        <v>43.58</v>
+        <v>49.56</v>
       </c>
       <c r="AE2" s="3" t="n">
         <f aca="false">SUM(AE7:AE22)</f>
@@ -1328,7 +1343,7 @@
       </c>
       <c r="AK2" s="3" t="n">
         <f aca="false">SUM(AK7:AK22)</f>
-        <v>2037.50011</v>
+        <v>2044.65773</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,7 +1352,7 @@
       </c>
       <c r="I3" s="4" t="n">
         <f aca="false">TotalCost/BoardQty</f>
-        <v>13.007801</v>
+        <v>13.539265</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1596,7 @@
         <v>17.61</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>16296</v>
+        <v>16272</v>
       </c>
       <c r="L8" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K8="",G8,K8),{0,1,10,50,100,250,500,1000,2500,5000},{0,0.74,0.651,0.5868,0.5612,0.5102,0.45918,0.40816,0.3699,0.35714}),"")</f>
@@ -1601,7 +1616,7 @@
         <v>27</v>
       </c>
       <c r="AB8" s="0" t="n">
-        <v>6394</v>
+        <v>6344</v>
       </c>
       <c r="AD8" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(AC8="",G8,AC8),{0,1,10,100,500,1000,5000,10000},{0,0.65,0.587,0.51,0.408,0.383,0.357,0.339}),"")</f>
@@ -1644,7 +1659,7 @@
         <v>3.18</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>85749</v>
+        <v>85705</v>
       </c>
       <c r="L9" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K9="",G9,K9),{0,1,10,25,50,100,250,500,1200,2400,6000,8400,12000,30000,60000},{0,0.46,0.437,0.3744,0.318,0.3056,0.27444,0.26196,0.19845,0.18144,0.1701,0.15876,0.15309,0.15082,0.14742}),"")</f>
@@ -1678,7 +1693,7 @@
         <v>27</v>
       </c>
       <c r="V9" s="0" t="n">
-        <v>35303</v>
+        <v>35130</v>
       </c>
       <c r="X9" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(W9="",G9,W9),{0,1,10,100,500,1200,2400},{0,0.46,0.318,0.273,0.261,0.229,0.209}),"")</f>
@@ -1741,7 +1756,7 @@
         <v>12.948</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>36230</v>
+        <v>36068</v>
       </c>
       <c r="L10" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K10="",G10,K10),{0,1,10,25,50,100,250,500,1000,2500},{0,0.6,0.463,0.4316,0.3926,0.3533,0.29832,0.2826,0.2512,0.20881}),"")</f>
@@ -1768,31 +1783,105 @@
       <c r="D11" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="G11" s="0" t="n">
         <f aca="false">BoardQty*2</f>
         <v>20</v>
       </c>
       <c r="H11" s="12" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+2)))</f>
-        <v>0</v>
+        <v>0.265732</v>
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">IFERROR(G11*H11,"")</f>
-        <v>0</v>
+        <v>5.31464</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>3399</v>
+      </c>
+      <c r="L11" s="12" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(K11="",G11,K11),{0,1,100,500},{0,0.35,0.3159,0.2673}),"")</f>
+        <v>0.35</v>
+      </c>
+      <c r="M11" s="12" t="n">
+        <f aca="false">IFERROR(IF(K11="",G11,K11)*L11,"")</f>
+        <v>7</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>813</v>
+      </c>
+      <c r="R11" s="12" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(Q11="",G11,Q11),{0,1,10,50,100,250,1000,3000,7000},{0,0.357881,0.265732,0.2218005,0.201442,0.19287,0.1832265,0.180012,0.175726}),"")</f>
+        <v>0.265732</v>
+      </c>
+      <c r="S11" s="12" t="n">
+        <f aca="false">IFERROR(IF(Q11="",G11,Q11)*R11,"")</f>
+        <v>5.31464</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>1025</v>
+      </c>
+      <c r="X11" s="12" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(W11="",G11,W11),{0,1,10,25,50,100},{0,0.36,0.299,0.249,0.208,0.189}),"")</f>
+        <v>0.299</v>
+      </c>
+      <c r="Y11" s="12" t="n">
+        <f aca="false">IFERROR(IF(W11="",G11,W11)*X11,"")</f>
+        <v>5.98</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="12" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(AI11="",G11,AI11),{0,1,5,125},{0,0.357881,0.357881,0.302163}),"")</f>
+        <v>0.357881</v>
+      </c>
+      <c r="AK11" s="12" t="n">
+        <f aca="false">IFERROR(IF(AI11="",G11,AI11)*AJ11,"")</f>
+        <v>7.15762</v>
+      </c>
+      <c r="AL11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM11" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -1818,7 +1907,7 @@
         <v>5.61</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="O12" s="13" t="s">
         <v>27</v>
@@ -1835,7 +1924,7 @@
         <v>2.89305</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="U12" s="13" t="s">
         <v>27</v>
@@ -1852,7 +1941,7 @@
         <v>5.72</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AA12" s="13" t="s">
         <v>27</v>
@@ -1869,7 +1958,7 @@
         <v>7.41</v>
       </c>
       <c r="AF12" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="AG12" s="13" t="s">
         <v>27</v>
@@ -1886,7 +1975,7 @@
         <v>7.13619</v>
       </c>
       <c r="AL12" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="AM12" s="13" t="s">
         <v>27</v>
@@ -1894,16 +1983,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">BoardQty*10</f>
@@ -1918,7 +2007,7 @@
         <v>0.6</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>822624</v>
+        <v>822400</v>
       </c>
       <c r="L13" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K13="",G13,K13),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.02,0.0148,0.011,0.009,0.00748,0.0064,0.00502,0.00367,0.00335,0.00319,0.00303,0.00219}),"")</f>
@@ -1929,7 +2018,7 @@
         <v>0.9</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="O13" s="13" t="s">
         <v>27</v>
@@ -1946,13 +2035,13 @@
         <v>0.62147</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="U13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>1465</v>
+        <v>1180</v>
       </c>
       <c r="X13" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(W13="",G13,W13),{0,1,10,100,1000,4000},{0,0.1,0.013,0.006,0.004,0.003}),"")</f>
@@ -1963,7 +2052,7 @@
         <v>0.6</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AA13" s="13" t="s">
         <v>27</v>
@@ -1980,7 +2069,7 @@
         <v>1.1</v>
       </c>
       <c r="AF13" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AG13" s="13" t="s">
         <v>27</v>
@@ -1997,7 +2086,7 @@
         <v>2016.563</v>
       </c>
       <c r="AL13" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="AM13" s="13" t="s">
         <v>27</v>
@@ -2005,16 +2094,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -2040,7 +2129,7 @@
         <v>4.51</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="O14" s="13" t="s">
         <v>27</v>
@@ -2057,7 +2146,7 @@
         <v>3.3</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AA14" s="13" t="s">
         <v>27</v>
@@ -2074,7 +2163,7 @@
         <v>1.47</v>
       </c>
       <c r="AF14" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="AG14" s="13" t="s">
         <v>27</v>
@@ -2082,17 +2171,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G15" s="0" t="n">
-        <f aca="false">BoardQty*3</f>
-        <v>30</v>
+        <f aca="false">BoardQty*4</f>
+        <v>40</v>
       </c>
       <c r="H15" s="12" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+2)))</f>
@@ -2105,16 +2194,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -2140,7 +2229,7 @@
         <v>13.98</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="O16" s="13" t="s">
         <v>27</v>
@@ -2160,7 +2249,7 @@
         <v>13.80092</v>
       </c>
       <c r="AL16" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="AM16" s="13" t="s">
         <v>27</v>
@@ -2168,16 +2257,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">BoardQty*4</f>
@@ -2192,7 +2281,7 @@
         <v>0.222872</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>1601626</v>
+        <v>1571416</v>
       </c>
       <c r="L17" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K17="",G17,K17),{0,1,10,25,50,100,250,500,1000,5000,10000,25000,50000,125000},{0,0.1,0.01,0.0072,0.0054,0.004,0.00308,0.00244,0.0018,0.00129,0.00112,0.00099,0.0009,0.00089}),"")</f>
@@ -2203,7 +2292,7 @@
         <v>0.288</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O17" s="13" t="s">
         <v>27</v>
@@ -2220,13 +2309,13 @@
         <v>0.222872</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="U17" s="13" t="s">
         <v>27</v>
       </c>
       <c r="V17" s="0" t="n">
-        <v>177057</v>
+        <v>171993</v>
       </c>
       <c r="X17" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(W17="",G17,W17),{0,1,10,100,1000,5000},{0,0.1,0.008,0.002,0.001,0.001}),"")</f>
@@ -2237,7 +2326,7 @@
         <v>0.32</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="AA17" s="13" t="s">
         <v>27</v>
@@ -2254,7 +2343,7 @@
         <v>0.28</v>
       </c>
       <c r="AF17" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="AG17" s="13" t="s">
         <v>27</v>
@@ -2262,16 +2351,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -2297,7 +2386,7 @@
         <v>3.58</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O18" s="13" t="s">
         <v>27</v>
@@ -2314,7 +2403,7 @@
         <v>3.47</v>
       </c>
       <c r="Z18" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="AA18" s="13" t="s">
         <v>27</v>
@@ -2328,16 +2417,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -2352,7 +2441,7 @@
         <v>21.2</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>29959</v>
+        <v>29915</v>
       </c>
       <c r="L19" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K19="",G19,K19),{0,1,25,100,250,500,1000,2000},{0,2.12,2.05,1.98,1.78,1.6,1.55,1.55}),"")</f>
@@ -2363,7 +2452,7 @@
         <v>21.2</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="O19" s="13" t="s">
         <v>27</v>
@@ -2380,13 +2469,13 @@
         <v>25.60885</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="U19" s="13" t="s">
         <v>27</v>
       </c>
       <c r="V19" s="0" t="n">
-        <v>3021</v>
+        <v>3016</v>
       </c>
       <c r="X19" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(W19="",G19,W19),{0,1,25,100,250,500},{0,2.12,2.05,1.98,1.78,1.61}),"")</f>
@@ -2397,7 +2486,7 @@
         <v>21.2</v>
       </c>
       <c r="Z19" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AA19" s="13" t="s">
         <v>27</v>
@@ -2408,16 +2497,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">BoardQty*1</f>
@@ -2432,7 +2521,7 @@
         <v>0.527178</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>78622</v>
+        <v>74587</v>
       </c>
       <c r="L20" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K20="",G20,K20),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.1,0.078,0.0696,0.0512,0.0442,0.03488,0.02946,0.02482,0.02256,0.02045,0.01974,0.01833,0.01812}),"")</f>
@@ -2443,13 +2532,13 @@
         <v>0.78</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="O20" s="13" t="s">
         <v>27</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>474</v>
+        <v>104</v>
       </c>
       <c r="R20" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(Q20="",G20,Q20),{0,1,100,500,1000,2000,4000,20000,40000},{0,0.0527178,0.0527178,0.03760965,0.0330022,0.02925195,0.02560885,0.02196575,0.02153715}),"")</f>
@@ -2460,13 +2549,13 @@
         <v>0.527178</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="U20" s="13" t="s">
         <v>27</v>
       </c>
       <c r="V20" s="0" t="n">
-        <v>13531</v>
+        <v>13526</v>
       </c>
       <c r="X20" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(W20="",G20,W20),{0,1,10,100,1000,4000,8000,24000},{0,0.1,0.067,0.033,0.028,0.02,0.019,0.018}),"")</f>
@@ -2477,7 +2566,7 @@
         <v>0.67</v>
       </c>
       <c r="Z20" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AA20" s="13" t="s">
         <v>27</v>
@@ -2491,16 +2580,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">BoardQty*2</f>
@@ -2515,7 +2604,7 @@
         <v>0.16</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>382014</v>
+        <v>381989</v>
       </c>
       <c r="L21" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K21="",G21,K21),{0,1,10,25,50,100,250,500,1000,5000,10000,25000,50000,125000},{0,0.1,0.01,0.0072,0.0054,0.004,0.00308,0.00244,0.0018,0.00129,0.00112,0.00099,0.0009,0.00089}),"")</f>
@@ -2526,7 +2615,7 @@
         <v>0.2</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="O21" s="13" t="s">
         <v>27</v>
@@ -2546,7 +2635,7 @@
         <v>0.16</v>
       </c>
       <c r="Z21" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="AA21" s="13" t="s">
         <v>27</v>
@@ -2557,16 +2646,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">BoardQty*2</f>
@@ -2581,7 +2670,7 @@
         <v>4.13599</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>82840</v>
+        <v>66840</v>
       </c>
       <c r="L22" s="12" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K22="",G22,K22),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000,100000},{0,0.47,0.326,0.2672,0.2282,0.1956,0.163,0.14672,0.12389,0.09639,0.09072,0.08789,0.08505,0.07371}),"")</f>
@@ -2592,7 +2681,7 @@
         <v>6.52</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="O22" s="13" t="s">
         <v>27</v>
@@ -2609,7 +2698,7 @@
         <v>4.13599</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="U22" s="13" t="s">
         <v>27</v>
@@ -2626,7 +2715,7 @@
         <v>4.96</v>
       </c>
       <c r="Z22" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="AA22" s="13" t="s">
         <v>27</v>
@@ -2643,7 +2732,7 @@
         <v>6.6</v>
       </c>
       <c r="AF22" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="AG22" s="13" t="s">
         <v>27</v>
@@ -3723,343 +3812,383 @@
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AJ11">
+    <cfRule type="cellIs" priority="16" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AJ12">
-    <cfRule type="cellIs" priority="16" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="17" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ13">
-    <cfRule type="cellIs" priority="17" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="18" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ16">
-    <cfRule type="cellIs" priority="18" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="19" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H16</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AK11">
+    <cfRule type="cellIs" priority="20" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AK12">
-    <cfRule type="cellIs" priority="19" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="21" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK13">
-    <cfRule type="cellIs" priority="20" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="22" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK16">
-    <cfRule type="cellIs" priority="21" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="23" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" priority="22" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="24" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L11">
+    <cfRule type="cellIs" priority="25" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="cellIs" priority="23" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="26" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" priority="24" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="27" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" priority="25" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="28" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="cellIs" priority="26" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="29" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" priority="27" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="30" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" priority="28" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="31" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="cellIs" priority="29" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="32" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" priority="30" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="33" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" priority="31" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="34" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" priority="32" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="35" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" priority="33" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="36" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" priority="34" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="37" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" priority="35" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="38" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" priority="36" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="39" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M11">
+    <cfRule type="cellIs" priority="40" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" priority="37" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="41" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" priority="38" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="42" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" priority="39" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="43" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" priority="40" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="44" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="cellIs" priority="41" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="45" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" priority="42" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="46" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="cellIs" priority="43" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="47" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
-    <cfRule type="cellIs" priority="44" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="48" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" priority="45" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="49" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="cellIs" priority="46" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="50" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" priority="47" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="51" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" priority="48" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="52" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" priority="49" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="53" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="cellIs" priority="54" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R12">
-    <cfRule type="cellIs" priority="50" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="55" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R13">
-    <cfRule type="cellIs" priority="51" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="56" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17">
-    <cfRule type="cellIs" priority="52" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="57" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19">
-    <cfRule type="cellIs" priority="53" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="58" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R20">
-    <cfRule type="cellIs" priority="54" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="59" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="cellIs" priority="55" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="60" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9">
-    <cfRule type="cellIs" priority="56" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="61" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="cellIs" priority="62" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S12">
-    <cfRule type="cellIs" priority="57" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="63" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13">
-    <cfRule type="cellIs" priority="58" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="64" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17">
-    <cfRule type="cellIs" priority="59" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="65" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19">
-    <cfRule type="cellIs" priority="60" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="66" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="cellIs" priority="61" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="67" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="cellIs" priority="62" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="68" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" priority="63" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="69" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X11">
+    <cfRule type="cellIs" priority="70" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="X12">
-    <cfRule type="cellIs" priority="64" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="71" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="cellIs" priority="65" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="72" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X14">
-    <cfRule type="cellIs" priority="66" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="73" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X17">
-    <cfRule type="cellIs" priority="67" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="74" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X18">
-    <cfRule type="cellIs" priority="68" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="75" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X19">
-    <cfRule type="cellIs" priority="69" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="76" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X20">
-    <cfRule type="cellIs" priority="70" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="77" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X21">
-    <cfRule type="cellIs" priority="71" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="78" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X22">
-    <cfRule type="cellIs" priority="72" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="79" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X9">
-    <cfRule type="cellIs" priority="73" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="80" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" priority="81" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Y12">
-    <cfRule type="cellIs" priority="74" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="82" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y13">
-    <cfRule type="cellIs" priority="75" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="83" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y14">
-    <cfRule type="cellIs" priority="76" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="84" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y17">
-    <cfRule type="cellIs" priority="77" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="85" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y18">
-    <cfRule type="cellIs" priority="78" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="86" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y19">
-    <cfRule type="cellIs" priority="79" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="87" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y20">
-    <cfRule type="cellIs" priority="80" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="88" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y21">
-    <cfRule type="cellIs" priority="81" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="89" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y22">
-    <cfRule type="cellIs" priority="82" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="90" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9">
-    <cfRule type="cellIs" priority="83" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="91" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4074,48 +4203,53 @@
     <hyperlink ref="AG9" r:id="rId9" display="Link"/>
     <hyperlink ref="AM9" r:id="rId10" display="Link"/>
     <hyperlink ref="O10" r:id="rId11" display="Link"/>
-    <hyperlink ref="O12" r:id="rId12" display="Link"/>
-    <hyperlink ref="U12" r:id="rId13" display="Link"/>
-    <hyperlink ref="AA12" r:id="rId14" display="Link"/>
-    <hyperlink ref="AG12" r:id="rId15" display="Link"/>
-    <hyperlink ref="AM12" r:id="rId16" display="Link"/>
-    <hyperlink ref="O13" r:id="rId17" display="Link"/>
-    <hyperlink ref="U13" r:id="rId18" display="Link"/>
-    <hyperlink ref="AA13" r:id="rId19" display="Link"/>
-    <hyperlink ref="AG13" r:id="rId20" display="Link"/>
-    <hyperlink ref="AM13" r:id="rId21" display="Link"/>
-    <hyperlink ref="O14" r:id="rId22" display="Link"/>
-    <hyperlink ref="AA14" r:id="rId23" display="Link"/>
-    <hyperlink ref="AG14" r:id="rId24" display="Link"/>
-    <hyperlink ref="O16" r:id="rId25" display="Link"/>
-    <hyperlink ref="AG16" r:id="rId26" display="Link"/>
-    <hyperlink ref="AM16" r:id="rId27" display="Link"/>
-    <hyperlink ref="O17" r:id="rId28" display="Link"/>
-    <hyperlink ref="U17" r:id="rId29" display="Link"/>
-    <hyperlink ref="AA17" r:id="rId30" display="Link"/>
-    <hyperlink ref="AG17" r:id="rId31" display="Link"/>
-    <hyperlink ref="O18" r:id="rId32" display="Link"/>
-    <hyperlink ref="AA18" r:id="rId33" display="Link"/>
-    <hyperlink ref="AG18" r:id="rId34" display="Link"/>
-    <hyperlink ref="AM18" r:id="rId35" display="Link"/>
-    <hyperlink ref="O19" r:id="rId36" display="Link"/>
-    <hyperlink ref="U19" r:id="rId37" display="Link"/>
-    <hyperlink ref="AA19" r:id="rId38" display="Link"/>
-    <hyperlink ref="AM19" r:id="rId39" display="Link"/>
-    <hyperlink ref="O20" r:id="rId40" display="Link"/>
-    <hyperlink ref="U20" r:id="rId41" display="Link"/>
-    <hyperlink ref="AA20" r:id="rId42" display="Link"/>
-    <hyperlink ref="AG20" r:id="rId43" display="Link"/>
-    <hyperlink ref="AM20" r:id="rId44" display="Link"/>
-    <hyperlink ref="O21" r:id="rId45" display="Link"/>
-    <hyperlink ref="U21" r:id="rId46" display="Link"/>
-    <hyperlink ref="AA21" r:id="rId47" display="Link"/>
-    <hyperlink ref="AG21" r:id="rId48" display="Link"/>
-    <hyperlink ref="O22" r:id="rId49" display="Link"/>
-    <hyperlink ref="U22" r:id="rId50" display="Link"/>
-    <hyperlink ref="AA22" r:id="rId51" display="Link"/>
-    <hyperlink ref="AG22" r:id="rId52" display="Link"/>
-    <hyperlink ref="AM22" r:id="rId53" display="Link"/>
+    <hyperlink ref="O11" r:id="rId12" display="Link"/>
+    <hyperlink ref="U11" r:id="rId13" display="Link"/>
+    <hyperlink ref="AA11" r:id="rId14" display="Link"/>
+    <hyperlink ref="AG11" r:id="rId15" display="Link"/>
+    <hyperlink ref="AM11" r:id="rId16" display="Link"/>
+    <hyperlink ref="O12" r:id="rId17" display="Link"/>
+    <hyperlink ref="U12" r:id="rId18" display="Link"/>
+    <hyperlink ref="AA12" r:id="rId19" display="Link"/>
+    <hyperlink ref="AG12" r:id="rId20" display="Link"/>
+    <hyperlink ref="AM12" r:id="rId21" display="Link"/>
+    <hyperlink ref="O13" r:id="rId22" display="Link"/>
+    <hyperlink ref="U13" r:id="rId23" display="Link"/>
+    <hyperlink ref="AA13" r:id="rId24" display="Link"/>
+    <hyperlink ref="AG13" r:id="rId25" display="Link"/>
+    <hyperlink ref="AM13" r:id="rId26" display="Link"/>
+    <hyperlink ref="O14" r:id="rId27" display="Link"/>
+    <hyperlink ref="AA14" r:id="rId28" display="Link"/>
+    <hyperlink ref="AG14" r:id="rId29" display="Link"/>
+    <hyperlink ref="O16" r:id="rId30" display="Link"/>
+    <hyperlink ref="AG16" r:id="rId31" display="Link"/>
+    <hyperlink ref="AM16" r:id="rId32" display="Link"/>
+    <hyperlink ref="O17" r:id="rId33" display="Link"/>
+    <hyperlink ref="U17" r:id="rId34" display="Link"/>
+    <hyperlink ref="AA17" r:id="rId35" display="Link"/>
+    <hyperlink ref="AG17" r:id="rId36" display="Link"/>
+    <hyperlink ref="O18" r:id="rId37" display="Link"/>
+    <hyperlink ref="AA18" r:id="rId38" display="Link"/>
+    <hyperlink ref="AG18" r:id="rId39" display="Link"/>
+    <hyperlink ref="AM18" r:id="rId40" display="Link"/>
+    <hyperlink ref="O19" r:id="rId41" display="Link"/>
+    <hyperlink ref="U19" r:id="rId42" display="Link"/>
+    <hyperlink ref="AA19" r:id="rId43" display="Link"/>
+    <hyperlink ref="AM19" r:id="rId44" display="Link"/>
+    <hyperlink ref="O20" r:id="rId45" display="Link"/>
+    <hyperlink ref="U20" r:id="rId46" display="Link"/>
+    <hyperlink ref="AA20" r:id="rId47" display="Link"/>
+    <hyperlink ref="AG20" r:id="rId48" display="Link"/>
+    <hyperlink ref="AM20" r:id="rId49" display="Link"/>
+    <hyperlink ref="O21" r:id="rId50" display="Link"/>
+    <hyperlink ref="U21" r:id="rId51" display="Link"/>
+    <hyperlink ref="AA21" r:id="rId52" display="Link"/>
+    <hyperlink ref="AG21" r:id="rId53" display="Link"/>
+    <hyperlink ref="O22" r:id="rId54" display="Link"/>
+    <hyperlink ref="U22" r:id="rId55" display="Link"/>
+    <hyperlink ref="AA22" r:id="rId56" display="Link"/>
+    <hyperlink ref="AG22" r:id="rId57" display="Link"/>
+    <hyperlink ref="AM22" r:id="rId58" display="Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4124,6 +4258,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId54"/>
+  <legacyDrawing r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>